<commit_message>
Completed Project By Adding Multiple Workflows for Download / Process and Linked Between them
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xune\Documents\UiPath\Hash_UIP_Advanced\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xune\Documents\UiPath\Yearly_Report_UIP_Advanced\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24757D2-2681-480D-8CAE-905F20EDBF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E61AA4-3AD4-4090-B713-0C0DAB71B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="2640" windowWidth="10740" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15060" yWindow="2640" windowWidth="10740" windowHeight="10335" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>CredentialName</t>
+  </si>
+  <si>
+    <t>DownloadPath</t>
   </si>
 </sst>
 </file>
@@ -540,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2790,8 +2793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2838,7 +2841,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>